<commit_message>
Update from New HDD
</commit_message>
<xml_diff>
--- a/GSMLiftSquare/Project Outputs/BOM/Bill of Materials-GSMLiftSquare(Production_Last).xlsx
+++ b/GSMLiftSquare/Project Outputs/BOM/Bill of Materials-GSMLiftSquare(Production_Last).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t>Comment</t>
   </si>
@@ -49,6 +49,15 @@
     <t>SMD_0402_RESC1005X37N</t>
   </si>
   <si>
+    <t>1N4731(A) 4.3V</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>PTH_HDRV02W64P254_1X02</t>
+  </si>
+  <si>
     <t>10k</t>
   </si>
   <si>
@@ -206,6 +215,15 @@
   </si>
   <si>
     <t>SMD_CON_ANTENNA_SMA_RIGHT_ANGLE</t>
+  </si>
+  <si>
+    <t>SMBJ5.0CA</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>SMD_DO214AC_SMB</t>
   </si>
   <si>
     <t>SPEAKER</t>
@@ -595,17 +613,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" customWidth="1"/>
+    <col min="5" max="5" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -670,27 +688,27 @@
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -707,72 +725,72 @@
         <v>18</v>
       </c>
       <c r="E6" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -939,10 +957,10 @@
         <v>55</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
@@ -950,13 +968,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>60</v>
@@ -1013,6 +1031,40 @@
         <v>69</v>
       </c>
       <c r="E24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>